<commit_message>
update folder data_processing and folder postman
</commit_message>
<xml_diff>
--- a/data_processing/ExlSqlScriptTransformation/MultiDF.xlsx
+++ b/data_processing/ExlSqlScriptTransformation/MultiDF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian199887/Downloads/github_francistan88/DSA/data_processing/ExlSqlScriptTransformation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56DE9A7-963E-F445-9C3D-2ECE3C200A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E661AC-38C9-1649-81F3-D5A509F000F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2020" yWindow="1140" windowWidth="32020" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -9554,8 +9554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U3669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3634" zoomScale="67" workbookViewId="0">
-      <selection activeCell="A3662" sqref="A3662"/>
+    <sheetView tabSelected="1" topLeftCell="A3640" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C3670" sqref="C3670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="48.59765625" defaultRowHeight="22" customHeight="1"/>

</xml_diff>